<commit_message>
combine all code in one
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Yue\OneDrive - The Ohio State University\research\OSU\2021-07 Differential privacy\privacy_ga\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DE537D-DE0D-4CF0-964C-0C95F006D609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47EC0A5B-4705-4D73-8AAF-9F9845AC8F97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="original" sheetId="4" r:id="rId1"/>
     <sheet name="set coverage" sheetId="2" r:id="rId2"/>
-    <sheet name="max coverage" sheetId="3" r:id="rId3"/>
+    <sheet name="max coverage" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="13">
   <si>
     <t>predicate</t>
   </si>
@@ -56,7 +56,16 @@
     <t>SMAPE</t>
   </si>
   <si>
-    <t>budget</t>
+    <t>\</t>
+  </si>
+  <si>
+    <t>penalized MAPE (objective)</t>
+  </si>
+  <si>
+    <t># of at-risk</t>
+  </si>
+  <si>
+    <t># of cells with at-risk</t>
   </si>
 </sst>
 </file>
@@ -66,10 +75,16 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -95,7 +110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -103,43 +118,12 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.000"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="18">
     <dxf>
       <numFmt numFmtId="164" formatCode="0.000"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -153,6 +137,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -166,6 +151,21 @@
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.000"/>
@@ -198,45 +198,58 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B4BA8DAF-2251-4B38-9CEF-F9F0C6EA0C1F}" name="Table2" displayName="Table2" ref="A1:C4" totalsRowShown="0" headerRowDxfId="21" dataDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B4BA8DAF-2251-4B38-9CEF-F9F0C6EA0C1F}" name="Table2" displayName="Table2" ref="A1:C4" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="A1:C4" xr:uid="{B4BA8DAF-2251-4B38-9CEF-F9F0C6EA0C1F}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{6B71ADEB-FDAE-4E40-A387-1B9FD5672593}" name="predicate" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{37CA440C-D3F1-493D-BC1E-A42480293A62}" name="risk-1" dataDxfId="18"/>
-    <tableColumn id="3" xr3:uid="{CB1FBEE8-7F44-4CFA-8FF3-31D6226794E1}" name="risk-2" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{6B71ADEB-FDAE-4E40-A387-1B9FD5672593}" name="predicate" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{37CA440C-D3F1-493D-BC1E-A42480293A62}" name="risk-1" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{CB1FBEE8-7F44-4CFA-8FF3-31D6226794E1}" name="risk-2" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8915D17A-4946-496A-96A4-A3105FE7CE4B}" name="Table1" displayName="Table1" ref="A1:F19" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
-  <autoFilter ref="A1:F19" xr:uid="{8915D17A-4946-496A-96A4-A3105FE7CE4B}"/>
-  <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{E93EEBB1-1ABA-4614-9534-4025000E8E79}" name="predicate" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{C5F5D603-C33F-4A2A-A480-A7622661CA75}" name="k" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{57777C39-F7C0-470F-9909-328B2220997B}" name="coverage" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{B1DB2743-AFA5-4F21-8A6A-E67F628495F4}" name="risk-1" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{03BB7C5E-3C1C-4E8B-BC60-8638B6C6016C}" name="risk-2" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{FE9DF15E-3794-4150-86AA-BE691124EBA1}" name="SMAPE" dataDxfId="9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{AA6A43C7-8A27-4791-8FD6-33C8F1924E0B}" name="Table5" displayName="Table5" ref="F1:H4" totalsRowShown="0">
+  <autoFilter ref="F1:H4" xr:uid="{AA6A43C7-8A27-4791-8FD6-33C8F1924E0B}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{037CE74B-7354-4D5F-B157-96B1ED2554D7}" name="k"/>
+    <tableColumn id="2" xr3:uid="{0F896A6D-F7D0-4458-9098-182F8E6E92E5}" name="# of at-risk"/>
+    <tableColumn id="3" xr3:uid="{72EB4576-DE88-43DE-8B03-6F93F1F24F30}" name="# of cells with at-risk"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{671D8403-D8AF-4EE3-B33D-F179EAAEE3CE}" name="Table14" displayName="Table14" ref="A1:G19" totalsRowShown="0" headerRowDxfId="8" dataDxfId="1">
-  <autoFilter ref="A1:G19" xr:uid="{671D8403-D8AF-4EE3-B33D-F179EAAEE3CE}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8915D17A-4946-496A-96A4-A3105FE7CE4B}" name="Table1" displayName="Table1" ref="A1:G19" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:G19" xr:uid="{8915D17A-4946-496A-96A4-A3105FE7CE4B}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{FD3BB01E-F47A-41F5-8BD6-3F38E6DEA826}" name="predicate" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{4A03B058-2E7E-4EC3-AB55-24080DB86909}" name="k" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{42A946DE-7510-4359-AE7B-24E80AEED93D}" name="coverage" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{64FFB0BC-B11A-4AC6-A1D0-AE11BE6553DE}" name="budget" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{B88DAAFD-A20A-4D18-A820-73A65EFE744B}" name="risk-1" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{8C802608-B747-4E3E-AC0C-0EA9B064CC29}" name="risk-2" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{830E7185-4C0C-4813-86A7-DBCF93F7867A}" name="SMAPE" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{E93EEBB1-1ABA-4614-9534-4025000E8E79}" name="predicate" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{C5F5D603-C33F-4A2A-A480-A7622661CA75}" name="k" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{57777C39-F7C0-470F-9909-328B2220997B}" name="coverage" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{0831C762-6C93-46E2-86CB-6BA872CA0846}" name="penalized MAPE (objective)" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{B1DB2743-AFA5-4F21-8A6A-E67F628495F4}" name="risk-1" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{03BB7C5E-3C1C-4E8B-BC60-8638B6C6016C}" name="risk-2" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{FE9DF15E-3794-4150-86AA-BE691124EBA1}" name="SMAPE" dataDxfId="0"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{59AF9031-C006-404D-8250-2B128413C736}" name="Table4" displayName="Table4" ref="A1:G55" totalsRowShown="0">
+  <autoFilter ref="A1:G55" xr:uid="{59AF9031-C006-404D-8250-2B128413C736}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{F5D0B863-4943-4DCE-A0AA-576A45FA1EF6}" name="predicate"/>
+    <tableColumn id="2" xr3:uid="{F5E81DB3-E4D4-487D-9DA8-6F21DD906986}" name="k"/>
+    <tableColumn id="3" xr3:uid="{2FD9EF43-7D1D-4E75-9218-B6FC0B9F80CF}" name="coverage"/>
+    <tableColumn id="6" xr3:uid="{782B4395-A5A1-43E9-982A-37E2CAEFAC07}" name="penalized MAPE (objective)" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{C43AB37C-685F-4E74-A37A-2C3D0E815DA8}" name="risk-1" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{C3A7C78B-879A-4F82-BBA2-13CB6A0187EE}" name="risk-2" dataDxfId="11"/>
+    <tableColumn id="7" xr3:uid="{6A2AA3C3-448F-497B-87BF-2195BBEF9EBD}" name="SMAPE" dataDxfId="10"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -503,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75B2CBC8-359E-4899-B9EA-5618EEAF0707}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -514,9 +527,11 @@
     <col min="1" max="1" width="33.08984375" customWidth="1"/>
     <col min="2" max="2" width="11.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.81640625" customWidth="1"/>
+    <col min="8" max="8" width="20.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -526,8 +541,17 @@
       <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="13" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -537,8 +561,11 @@
       <c r="C2" s="2">
         <v>8.60160965794768E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -548,8 +575,11 @@
       <c r="C3" s="2">
         <v>8.0985915492957694E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -559,58 +589,64 @@
       <c r="C4" s="2">
         <v>4.1750503018108599E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="F4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A301A827-400A-476B-933A-196F997189D0}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.81640625" customWidth="1"/>
-    <col min="2" max="2" width="17.08984375" customWidth="1"/>
+    <col min="1" max="1" width="32.90625" customWidth="1"/>
+    <col min="2" max="2" width="7.7265625" customWidth="1"/>
     <col min="3" max="3" width="10.1796875" customWidth="1"/>
-    <col min="4" max="4" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.54296875" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.36328125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -620,17 +656,20 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -641,32 +680,38 @@
         <v>1</v>
       </c>
       <c r="D2" s="2">
+        <v>9.3149596234555807E-2</v>
+      </c>
+      <c r="E2" s="2">
         <v>8.0435161409087005E-2</v>
       </c>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
       <c r="F2" s="2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="2">
         <v>8.7903062622176398E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1">
         <v>2</v>
       </c>
       <c r="D3" s="2">
+        <v>0.48891861406034998</v>
+      </c>
+      <c r="E3" s="2">
         <v>7.8067757973423205E-2</v>
       </c>
-      <c r="E3" s="2">
-        <v>0</v>
-      </c>
       <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
         <v>9.89236600009058E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1">
         <v>2</v>
@@ -675,32 +720,38 @@
         <v>1</v>
       </c>
       <c r="D4" s="2">
+        <v>0.16516249175566899</v>
+      </c>
+      <c r="E4" s="2">
         <v>5.0122813879065302E-2</v>
       </c>
-      <c r="E4" s="2">
-        <v>0</v>
-      </c>
       <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2">
         <v>0.15027313912694801</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1">
         <v>2</v>
       </c>
       <c r="D5" s="2">
+        <v>1.74883853991247</v>
+      </c>
+      <c r="E5" s="2">
         <v>4.80887763150687E-2</v>
       </c>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
       <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2">
         <v>0.17359379391952401</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="1"/>
       <c r="B6" s="1">
         <v>3</v>
@@ -709,32 +760,38 @@
         <v>1</v>
       </c>
       <c r="D6" s="2">
+        <v>0.357112905666638</v>
+      </c>
+      <c r="E6" s="2">
         <v>3.5476692399612798E-2</v>
       </c>
-      <c r="E6" s="2">
-        <v>0</v>
-      </c>
       <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2">
         <v>0.19592546474452699</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1">
         <v>2</v>
       </c>
       <c r="D7" s="2">
+        <v>4.0334536147400302</v>
+      </c>
+      <c r="E7" s="2">
         <v>3.4467426089457097E-2</v>
       </c>
-      <c r="E7" s="2">
-        <v>0</v>
-      </c>
       <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2">
         <v>0.23328700586173601</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
@@ -744,33 +801,39 @@
       <c r="C8" s="1">
         <v>1</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="2">
         <v>6.4764913656770104E-2</v>
       </c>
-      <c r="E8" s="2">
-        <v>0</v>
-      </c>
       <c r="F8" s="2">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2">
         <v>0.11930169960207899</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1">
         <v>2</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="2">
         <v>6.2010104661130397E-2</v>
       </c>
-      <c r="E9" s="2">
-        <v>0</v>
-      </c>
       <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2">
         <v>0.13333835735587199</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1">
         <v>2</v>
@@ -778,33 +841,39 @@
       <c r="C10" s="1">
         <v>1</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="2">
         <v>3.67138904511786E-2</v>
       </c>
-      <c r="E10" s="2">
-        <v>0</v>
-      </c>
       <c r="F10" s="2">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2">
         <v>0.197141106495476</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1">
         <v>2</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="2">
         <v>3.4605873141493299E-2</v>
       </c>
-      <c r="E11" s="2">
-        <v>0</v>
-      </c>
       <c r="F11" s="2">
+        <v>0</v>
+      </c>
+      <c r="G11" s="2">
         <v>0.217641389006546</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1">
         <v>3</v>
@@ -812,33 +881,39 @@
       <c r="C12" s="1">
         <v>1</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="2">
         <v>2.5116672512904701E-2</v>
       </c>
-      <c r="E12" s="2">
-        <v>0</v>
-      </c>
       <c r="F12" s="2">
+        <v>0</v>
+      </c>
+      <c r="G12" s="2">
         <v>0.249667094765121</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1">
         <v>2</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="2">
         <v>2.4226573865997299E-2</v>
       </c>
-      <c r="E13" s="2">
-        <v>0</v>
-      </c>
       <c r="F13" s="2">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
         <v>0.279596696908194</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
@@ -848,33 +923,39 @@
       <c r="C14" s="1">
         <v>1</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="2">
         <v>4.9598373005973598E-2</v>
       </c>
-      <c r="E14" s="2">
-        <v>0</v>
-      </c>
       <c r="F14" s="2">
+        <v>0</v>
+      </c>
+      <c r="G14" s="2">
         <v>0.102671771175548</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1">
         <v>2</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="2">
         <v>4.8851491861905502E-2</v>
       </c>
-      <c r="E15" s="2">
-        <v>0</v>
-      </c>
       <c r="F15" s="2">
+        <v>0</v>
+      </c>
+      <c r="G15" s="2">
         <v>0.13723396353404099</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1">
         <v>2</v>
@@ -882,33 +963,39 @@
       <c r="C16" s="1">
         <v>1</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="2">
         <v>3.3659502390868498E-2</v>
       </c>
-      <c r="E16" s="2">
-        <v>0</v>
-      </c>
       <c r="F16" s="2">
+        <v>0</v>
+      </c>
+      <c r="G16" s="2">
         <v>0.210972892843864</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1">
         <v>2</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="2">
         <v>3.2441068420356003E-2</v>
       </c>
-      <c r="E17" s="2">
-        <v>0</v>
-      </c>
       <c r="F17" s="2">
+        <v>0</v>
+      </c>
+      <c r="G17" s="2">
         <v>0.234710616589237</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1">
         <v>3</v>
@@ -916,33 +1003,40 @@
       <c r="C18" s="1">
         <v>1</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="2">
         <v>3.0641147798271502E-2</v>
       </c>
-      <c r="E18" s="2">
-        <v>0</v>
-      </c>
       <c r="F18" s="2">
+        <v>0</v>
+      </c>
+      <c r="G18" s="2">
         <v>0.26061472234037297</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1">
         <v>2</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="2">
         <v>2.85784333427084E-2</v>
       </c>
-      <c r="E19" s="2">
-        <v>0</v>
-      </c>
       <c r="F19" s="2">
+        <v>0</v>
+      </c>
+      <c r="G19" s="2">
         <v>0.26593610416325397</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <tableParts count="1">
@@ -952,268 +1046,606 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CA9A1EB-3013-40BD-AB5A-540B13BF4EC6}">
-  <dimension ref="A1:G19"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{836B1424-F873-4785-84D3-2D104A420DD8}">
+  <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.90625" customWidth="1"/>
-    <col min="3" max="4" width="13.7265625" customWidth="1"/>
+    <col min="1" max="1" width="32" customWidth="1"/>
+    <col min="3" max="3" width="10.26953125" customWidth="1"/>
+    <col min="4" max="4" width="26" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3">
-        <v>2</v>
-      </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="D3" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3">
-        <v>2</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="D4" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3">
-        <v>2</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3">
+      <c r="D6" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D7" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D9" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D10" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D12" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D13" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B14">
         <v>3</v>
       </c>
-      <c r="C6" s="3">
-        <v>1</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3">
-        <v>2</v>
-      </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D15" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D16" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E16" s="3">
+        <v>3.62264765445472E-2</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0</v>
+      </c>
+      <c r="G16" s="3">
+        <v>0.19206379642886201</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D18" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D19" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E19" s="3">
+        <v>3.5083197275066903E-2</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0</v>
+      </c>
+      <c r="G19" s="3">
+        <v>0.195411708763641</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="3">
-        <v>1</v>
-      </c>
-      <c r="C8" s="3">
-        <v>1</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3">
-        <v>2</v>
-      </c>
-      <c r="D9" s="3"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3">
-        <v>2</v>
-      </c>
-      <c r="C10" s="3">
-        <v>1</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3">
-        <v>2</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3">
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D21" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D22" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D24" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D25" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D27" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D28" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C29">
+        <v>2</v>
+      </c>
+      <c r="D29" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D30" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D31" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B32">
         <v>3</v>
       </c>
-      <c r="C12" s="3">
-        <v>1</v>
-      </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3">
-        <v>2</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D33" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D34" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E34" s="3">
+        <v>2.6046038507025498E-2</v>
+      </c>
+      <c r="F34" s="3">
+        <v>0</v>
+      </c>
+      <c r="G34" s="3">
+        <v>0.243413553361292</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D36" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+      <c r="G36" s="3"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D37" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E37" s="3">
+        <v>2.50304719361947E-2</v>
+      </c>
+      <c r="F37" s="3">
+        <v>0</v>
+      </c>
+      <c r="G37" s="3">
+        <v>0.24196482575418399</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="3">
-        <v>1</v>
-      </c>
-      <c r="C14" s="3">
-        <v>1</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3">
-        <v>2</v>
-      </c>
-      <c r="D15" s="3"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3">
-        <v>2</v>
-      </c>
-      <c r="C16" s="3">
-        <v>1</v>
-      </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" s="3"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3">
-        <v>2</v>
-      </c>
-      <c r="D17" s="3"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3">
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+      <c r="G38" s="3"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D39" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="E39" s="3"/>
+      <c r="F39" s="3"/>
+      <c r="G39" s="3"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D40" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D42" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D43" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B44">
+        <v>2</v>
+      </c>
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D45" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D46" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+      <c r="G46" s="3"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C47">
+        <v>2</v>
+      </c>
+      <c r="D47" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="D48" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3"/>
+      <c r="G48" s="3"/>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="D49" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B50">
         <v>3</v>
       </c>
-      <c r="C18" s="3">
-        <v>1</v>
-      </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3">
-        <v>2</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="D51" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="D52" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E52" s="3">
+        <v>3.0910642033521101E-2</v>
+      </c>
+      <c r="F52" s="3">
+        <v>0</v>
+      </c>
+      <c r="G52" s="3">
+        <v>0.23930655149765401</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="C53">
+        <v>2</v>
+      </c>
+      <c r="D53" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="E53" s="3"/>
+      <c r="F53" s="3"/>
+      <c r="G53" s="3"/>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="D54" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
+      <c r="G54" s="3"/>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="D55" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="E55" s="3">
+        <v>3.08428800905798E-2</v>
+      </c>
+      <c r="F55" s="3">
+        <v>0</v>
+      </c>
+      <c r="G55" s="3">
+        <v>0.23615446975283899</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>